<commit_message>
Added diet section and edited tranporttaion section
</commit_message>
<xml_diff>
--- a/api/python_vin_co2/transport_co2_data/Electricity_co2_countrywise.xlsx
+++ b/api/python_vin_co2/transport_co2_data/Electricity_co2_countrywise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KALPITA ROY\Desktop\Arjuna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFFA37B-D0DF-45E5-9762-B268ABF2E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B8F50C-40A8-4DE7-9436-FED61C5FD019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3168" yWindow="3168" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>country_code</t>
   </si>
@@ -43,16 +43,19 @@
     <t>United States</t>
   </si>
   <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
     <t>Germany</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>DEU</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +470,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.20300000000000001</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -475,9 +478,31 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
         <v>0.35</v>
       </c>
     </row>

</xml_diff>